<commit_message>
This is the first version of the review
</commit_message>
<xml_diff>
--- a/Foodies_Project_Review_Template.xlsx
+++ b/Foodies_Project_Review_Template.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TOP-TECH\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
   <si>
     <t>Review ID</t>
   </si>
@@ -46,24 +54,9 @@
     <t>RVW-001</t>
   </si>
   <si>
-    <t>2025-04-05</t>
-  </si>
-  <si>
     <t>Mariam ELhussiny</t>
   </si>
   <si>
-    <t>Planning</t>
-  </si>
-  <si>
-    <t>User Requirements Doc</t>
-  </si>
-  <si>
-    <t>Add roles for Admin &amp; Owner</t>
-  </si>
-  <si>
-    <t>Completed</t>
-  </si>
-  <si>
     <t>RVW-002</t>
   </si>
   <si>
@@ -76,28 +69,61 @@
     <t>RVW-003</t>
   </si>
   <si>
-    <t>2025-04-08</t>
-  </si>
-  <si>
     <t>RVW-004</t>
   </si>
   <si>
-    <t>2025-04-09</t>
-  </si>
-  <si>
-    <t>No action needed</t>
-  </si>
-  <si>
-    <t>Pending</t>
+    <t>Requirment 
+Gathering</t>
+  </si>
+  <si>
+    <t>SIQ</t>
+  </si>
+  <si>
+    <t>It is not required to send a verification mail to make an account ,just we can check if the account is used before or not</t>
+  </si>
+  <si>
+    <t>Approved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin should add menus,add new items ,
+delete items,add and delete offers and promotions, not delete users </t>
+  </si>
+  <si>
+    <t>Items should be categrized</t>
+  </si>
+  <si>
+    <t>The question is not clear enough</t>
+  </si>
+  <si>
+    <t>SIQ_FEAT001_001</t>
+  </si>
+  <si>
+    <t>SIQ_FEAT002_002</t>
+  </si>
+  <si>
+    <t>SIQ_FEAT004_001</t>
+  </si>
+  <si>
+    <t>SIQ_FEAT005_001</t>
+  </si>
+  <si>
+    <t>No need for email verification to create 
+an account.</t>
+  </si>
+  <si>
+    <t>Admin can not delete users</t>
+  </si>
+  <si>
+    <t>Items should be categorized</t>
+  </si>
+  <si>
+    <t>The question is not enough</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -105,40 +131,41 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
       <sz val="16"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="20"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="17"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="16"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="14"/>
       <color indexed="13"/>
       <name val="Helvetica Neue"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,8 +184,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -167,47 +200,32 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="10"/>
-      </left>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="10"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
+      <left style="thin">
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -215,29 +233,86 @@
       <left style="thin">
         <color indexed="11"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
       <top style="thin">
         <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -249,10 +324,10 @@
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -263,107 +338,106 @@
       <right style="thin">
         <color indexed="11"/>
       </right>
-      <top style="medium">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="32">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="11">
     <dxf>
       <font>
-        <b val="1"/>
-        <color rgb="00000000"/>
+        <color rgb="FF000000"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="18"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
-        <color rgb="00000000"/>
+        <color rgb="FF000000"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="17"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="ff000000"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="16"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
       </font>
       <fill>
         <patternFill patternType="solid">
@@ -374,68 +448,129 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="ff000000"/>
+        <b/>
+        <color rgb="FF000000"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="14"/>
-          <bgColor indexed="16"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="ff000000"/>
+        <b/>
+        <color rgb="FF000000"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="14"/>
-          <bgColor indexed="17"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="ff000000"/>
+        <b/>
+        <color rgb="FF000000"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="14"/>
-          <bgColor indexed="18"/>
-        </patternFill>
-      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF000000"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="fff9b074"/>
-      <rgbColor rgb="fff79646"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="fffcdabe"/>
-      <rgbColor rgb="ff111111"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFF9B074"/>
+      <rgbColor rgb="FFF79646"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FFFCDABE"/>
+      <rgbColor rgb="FF111111"/>
       <rgbColor rgb="00000000"/>
-      <rgbColor rgb="e5fffc98"/>
-      <rgbColor rgb="e588ccff"/>
-      <rgbColor rgb="e5afe489"/>
-      <rgbColor rgb="e5ff9781"/>
-      <rgbColor rgb="ff9bbb59"/>
+      <rgbColor rgb="E5FFFC98"/>
+      <rgbColor rgb="E588CCFF"/>
+      <rgbColor rgb="E5AFE489"/>
+      <rgbColor rgb="E5FF9781"/>
+      <rgbColor rgb="FF9BBB59"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -561,7 +696,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -570,7 +705,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -579,7 +714,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -653,7 +788,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -661,7 +796,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -679,7 +814,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -708,7 +843,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -733,7 +868,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -758,7 +893,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -783,7 +918,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -808,7 +943,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -833,7 +968,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -858,7 +993,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -883,7 +1018,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -908,7 +1043,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -921,9 +1056,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -938,7 +1079,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="38000"/>
             </a:srgbClr>
@@ -946,7 +1087,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -964,7 +1105,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -989,7 +1130,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1014,7 +1155,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1039,7 +1180,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1064,7 +1205,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1089,7 +1230,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1114,7 +1255,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1139,7 +1280,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1164,7 +1305,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1189,7 +1330,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1202,9 +1343,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1218,7 +1365,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1236,7 +1383,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1265,7 +1412,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1290,7 +1437,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1315,7 +1462,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1340,7 +1487,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1365,7 +1512,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1390,7 +1537,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1415,7 +1562,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1440,7 +1587,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1465,7 +1612,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1478,337 +1625,391 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="21.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21.45" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.6875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6797" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.4062" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.0703" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.2266" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="35.9062" style="1" customWidth="1"/>
-    <col min="9" max="9" width="32.9062" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6016" style="1" customWidth="1"/>
-    <col min="11" max="15" width="11.6719" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="29.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="44.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.21875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" style="1" customWidth="1"/>
+    <col min="11" max="15" width="11.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="8.88671875" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="26.8" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:15" ht="26.85" customHeight="1">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="3">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="4">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="5">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="4">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="4">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="6">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="4">
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="4">
+      <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="7">
+      <c r="J1" s="9" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="8"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
     </row>
-    <row r="2" ht="26.8" customHeight="1">
-      <c r="A2" t="s" s="11">
+    <row r="2" spans="1:15" ht="70.2" customHeight="1">
+      <c r="A2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s" s="12">
+      <c r="B2" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s" s="12">
+      <c r="D2" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="1:15" ht="79.2" customHeight="1">
+      <c r="A3" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s" s="12">
+      <c r="B3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" t="s" s="12">
+      <c r="C3" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" t="s" s="12">
+      <c r="K3" s="5"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" spans="1:15" ht="46.2" customHeight="1">
+      <c r="A4" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="J2" t="s" s="14">
+      <c r="B4" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+    </row>
+    <row r="5" spans="1:15" ht="61.2" customHeight="1">
+      <c r="A5" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
+      <c r="B5" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="19"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
     </row>
-    <row r="3" ht="26.8" customHeight="1">
-      <c r="A3" t="s" s="15">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s" s="15">
-        <v>18</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" t="s" s="16">
-        <v>19</v>
-      </c>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
+    <row r="6" spans="1:15" s="23" customFormat="1" ht="65.400000000000006" customHeight="1">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
     </row>
-    <row r="4" ht="26.8" customHeight="1">
-      <c r="A4" t="s" s="15">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s" s="15">
-        <v>21</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" t="s" s="16">
-        <v>19</v>
-      </c>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
+    <row r="7" spans="1:15" ht="26.85" customHeight="1">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
     </row>
-    <row r="5" ht="26.8" customHeight="1">
-      <c r="A5" t="s" s="15">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s" s="15">
-        <v>23</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" t="s" s="15">
-        <v>24</v>
-      </c>
-      <c r="J5" t="s" s="16">
-        <v>25</v>
-      </c>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
+    <row r="8" spans="1:15" ht="26.85" customHeight="1">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
     </row>
-    <row r="6" ht="26.8" customHeight="1">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" t="s" s="16">
-        <v>25</v>
-      </c>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
+    <row r="9" spans="1:15" ht="26.85" customHeight="1">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
     </row>
-    <row r="7" ht="26.8" customHeight="1">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
+    <row r="10" spans="1:15" ht="26.85" customHeight="1">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
     </row>
-    <row r="8" ht="26.8" customHeight="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
+    <row r="11" spans="1:15" ht="26.85" customHeight="1">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
     </row>
-    <row r="9" ht="26.8" customHeight="1">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
+    <row r="12" spans="1:15" ht="26.85" customHeight="1">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
     </row>
-    <row r="10" ht="26.8" customHeight="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-    </row>
-    <row r="11" ht="26.8" customHeight="1">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-    </row>
-    <row r="12" ht="26.8" customHeight="1">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-    </row>
-    <row r="13" ht="26.8" customHeight="1">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
+    <row r="13" spans="1:15" ht="26.85" customHeight="1">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A13">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="1" stopIfTrue="1">
       <formula>NOT(ISBLANK(A1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D13">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="1" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="2" stopIfTrue="1">
       <formula>NOT(ISBLANK(D1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J13">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Approved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="1" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="0" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1818,7 +2019,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
This is the first version of SIQ reviewing
</commit_message>
<xml_diff>
--- a/Foodies_Project_Review_Template.xlsx
+++ b/Foodies_Project_Review_Template.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TOP-TECH\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
   <si>
     <t>Review ID</t>
   </si>
@@ -46,24 +54,9 @@
     <t>RVW-001</t>
   </si>
   <si>
-    <t>2025-04-05</t>
-  </si>
-  <si>
     <t>Mariam ELhussiny</t>
   </si>
   <si>
-    <t>Planning</t>
-  </si>
-  <si>
-    <t>User Requirements Doc</t>
-  </si>
-  <si>
-    <t>Add roles for Admin &amp; Owner</t>
-  </si>
-  <si>
-    <t>Completed</t>
-  </si>
-  <si>
     <t>RVW-002</t>
   </si>
   <si>
@@ -76,28 +69,61 @@
     <t>RVW-003</t>
   </si>
   <si>
-    <t>2025-04-08</t>
-  </si>
-  <si>
     <t>RVW-004</t>
   </si>
   <si>
-    <t>2025-04-09</t>
-  </si>
-  <si>
-    <t>No action needed</t>
-  </si>
-  <si>
-    <t>Pending</t>
+    <t>Requirment 
+Gathering</t>
+  </si>
+  <si>
+    <t>SIQ</t>
+  </si>
+  <si>
+    <t>It is not required to send a verification mail to make an account ,just we can check if the account is used before or not</t>
+  </si>
+  <si>
+    <t>Approved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin should add menus,add new items ,
+delete items,add and delete offers and promotions, not delete users </t>
+  </si>
+  <si>
+    <t>Items should be categrized</t>
+  </si>
+  <si>
+    <t>The question is not clear enough</t>
+  </si>
+  <si>
+    <t>SIQ_FEAT001_001</t>
+  </si>
+  <si>
+    <t>SIQ_FEAT002_002</t>
+  </si>
+  <si>
+    <t>SIQ_FEAT004_001</t>
+  </si>
+  <si>
+    <t>SIQ_FEAT005_001</t>
+  </si>
+  <si>
+    <t>No need for email verification to create 
+an account.</t>
+  </si>
+  <si>
+    <t>Admin can not delete users</t>
+  </si>
+  <si>
+    <t>Items should be categorized</t>
+  </si>
+  <si>
+    <t>The question is not enough</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -105,40 +131,41 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
       <sz val="16"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="20"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="17"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="16"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="14"/>
       <color indexed="13"/>
       <name val="Helvetica Neue"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,8 +184,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -167,47 +200,32 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="10"/>
-      </left>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="10"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
+      <left style="thin">
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -215,29 +233,86 @@
       <left style="thin">
         <color indexed="11"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
       <top style="thin">
         <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -249,10 +324,10 @@
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -263,107 +338,106 @@
       <right style="thin">
         <color indexed="11"/>
       </right>
-      <top style="medium">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="32">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="11">
     <dxf>
       <font>
-        <b val="1"/>
-        <color rgb="00000000"/>
+        <color rgb="FF000000"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="18"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
-        <color rgb="00000000"/>
+        <color rgb="FF000000"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="17"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="ff000000"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="16"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
       </font>
       <fill>
         <patternFill patternType="solid">
@@ -374,68 +448,129 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="ff000000"/>
+        <b/>
+        <color rgb="FF000000"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="14"/>
-          <bgColor indexed="16"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="ff000000"/>
+        <b/>
+        <color rgb="FF000000"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="14"/>
-          <bgColor indexed="17"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="ff000000"/>
+        <b/>
+        <color rgb="FF000000"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="14"/>
-          <bgColor indexed="18"/>
-        </patternFill>
-      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF000000"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="fff9b074"/>
-      <rgbColor rgb="fff79646"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="fffcdabe"/>
-      <rgbColor rgb="ff111111"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFF9B074"/>
+      <rgbColor rgb="FFF79646"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FFFCDABE"/>
+      <rgbColor rgb="FF111111"/>
       <rgbColor rgb="00000000"/>
-      <rgbColor rgb="e5fffc98"/>
-      <rgbColor rgb="e588ccff"/>
-      <rgbColor rgb="e5afe489"/>
-      <rgbColor rgb="e5ff9781"/>
-      <rgbColor rgb="ff9bbb59"/>
+      <rgbColor rgb="E5FFFC98"/>
+      <rgbColor rgb="E588CCFF"/>
+      <rgbColor rgb="E5AFE489"/>
+      <rgbColor rgb="E5FF9781"/>
+      <rgbColor rgb="FF9BBB59"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -561,7 +696,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -570,7 +705,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -579,7 +714,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -653,7 +788,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -661,7 +796,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -679,7 +814,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -708,7 +843,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -733,7 +868,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -758,7 +893,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -783,7 +918,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -808,7 +943,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -833,7 +968,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -858,7 +993,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -883,7 +1018,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -908,7 +1043,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -921,9 +1056,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -938,7 +1079,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="38000"/>
             </a:srgbClr>
@@ -946,7 +1087,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -964,7 +1105,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -989,7 +1130,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1014,7 +1155,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1039,7 +1180,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1064,7 +1205,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1089,7 +1230,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1114,7 +1255,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1139,7 +1280,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1164,7 +1305,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1189,7 +1330,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1202,9 +1343,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1218,7 +1365,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1236,7 +1383,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1265,7 +1412,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1290,7 +1437,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1315,7 +1462,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1340,7 +1487,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1365,7 +1512,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1390,7 +1537,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1415,7 +1562,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1440,7 +1587,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1465,7 +1612,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1478,337 +1625,391 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="21.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21.45" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.6875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6797" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.4062" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.0703" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.2266" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="35.9062" style="1" customWidth="1"/>
-    <col min="9" max="9" width="32.9062" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6016" style="1" customWidth="1"/>
-    <col min="11" max="15" width="11.6719" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="29.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="44.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.21875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" style="1" customWidth="1"/>
+    <col min="11" max="15" width="11.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="8.88671875" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="26.8" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:15" ht="26.85" customHeight="1">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="3">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="4">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="5">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="4">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="4">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="6">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="4">
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="4">
+      <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="7">
+      <c r="J1" s="9" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="8"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
     </row>
-    <row r="2" ht="26.8" customHeight="1">
-      <c r="A2" t="s" s="11">
+    <row r="2" spans="1:15" ht="70.2" customHeight="1">
+      <c r="A2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s" s="12">
+      <c r="B2" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s" s="12">
+      <c r="D2" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="1:15" ht="79.2" customHeight="1">
+      <c r="A3" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s" s="12">
+      <c r="B3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" t="s" s="12">
+      <c r="C3" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" t="s" s="12">
+      <c r="K3" s="5"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" spans="1:15" ht="46.2" customHeight="1">
+      <c r="A4" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="J2" t="s" s="14">
+      <c r="B4" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+    </row>
+    <row r="5" spans="1:15" ht="61.2" customHeight="1">
+      <c r="A5" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
+      <c r="B5" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="19"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
     </row>
-    <row r="3" ht="26.8" customHeight="1">
-      <c r="A3" t="s" s="15">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s" s="15">
-        <v>18</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" t="s" s="16">
-        <v>19</v>
-      </c>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
+    <row r="6" spans="1:15" s="23" customFormat="1" ht="65.400000000000006" customHeight="1">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
     </row>
-    <row r="4" ht="26.8" customHeight="1">
-      <c r="A4" t="s" s="15">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s" s="15">
-        <v>21</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" t="s" s="16">
-        <v>19</v>
-      </c>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
+    <row r="7" spans="1:15" ht="26.85" customHeight="1">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
     </row>
-    <row r="5" ht="26.8" customHeight="1">
-      <c r="A5" t="s" s="15">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s" s="15">
-        <v>23</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" t="s" s="15">
-        <v>24</v>
-      </c>
-      <c r="J5" t="s" s="16">
-        <v>25</v>
-      </c>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
+    <row r="8" spans="1:15" ht="26.85" customHeight="1">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
     </row>
-    <row r="6" ht="26.8" customHeight="1">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" t="s" s="16">
-        <v>25</v>
-      </c>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
+    <row r="9" spans="1:15" ht="26.85" customHeight="1">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
     </row>
-    <row r="7" ht="26.8" customHeight="1">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
+    <row r="10" spans="1:15" ht="26.85" customHeight="1">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
     </row>
-    <row r="8" ht="26.8" customHeight="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
+    <row r="11" spans="1:15" ht="26.85" customHeight="1">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
     </row>
-    <row r="9" ht="26.8" customHeight="1">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
+    <row r="12" spans="1:15" ht="26.85" customHeight="1">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
     </row>
-    <row r="10" ht="26.8" customHeight="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-    </row>
-    <row r="11" ht="26.8" customHeight="1">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-    </row>
-    <row r="12" ht="26.8" customHeight="1">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-    </row>
-    <row r="13" ht="26.8" customHeight="1">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
+    <row r="13" spans="1:15" ht="26.85" customHeight="1">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A13">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="1" stopIfTrue="1">
       <formula>NOT(ISBLANK(A1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D13">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="1" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="2" stopIfTrue="1">
       <formula>NOT(ISBLANK(D1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J13">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Approved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="1" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="0" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1818,7 +2019,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
updated version of review template
this is an updated version of review template due to review crs
</commit_message>
<xml_diff>
--- a/Foodies_Project_Review_Template.xlsx
+++ b/Foodies_Project_Review_Template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TOP-TECH\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sagedwael/QA project/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9744396-7E9E-CD4A-8BBA-2C890EE8A00F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="89">
   <si>
     <t>Review ID</t>
   </si>
@@ -148,13 +149,154 @@
   </si>
   <si>
     <t>SIQ_FEAT007_001</t>
+  </si>
+  <si>
+    <t>RVW-010</t>
+  </si>
+  <si>
+    <t>Saged Wael</t>
+  </si>
+  <si>
+    <t>CRS</t>
+  </si>
+  <si>
+    <t>CRS_FEAT001_001</t>
+  </si>
+  <si>
+    <t>In requiremt description strong password is not clear enuogh</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t xml:space="preserve">you need to define what is strong password </t>
+  </si>
+  <si>
+    <t>RVW-011</t>
+  </si>
+  <si>
+    <t>CRS_FEAT002_001</t>
+  </si>
+  <si>
+    <t>CRS_FEAT002_002</t>
+  </si>
+  <si>
+    <t>RVW-012</t>
+  </si>
+  <si>
+    <t>RVW-013</t>
+  </si>
+  <si>
+    <t>RVW-014</t>
+  </si>
+  <si>
+    <t>CRS_FEAT003_001</t>
+  </si>
+  <si>
+    <t>CRS_FEAT002_003</t>
+  </si>
+  <si>
+    <t>RVW-015</t>
+  </si>
+  <si>
+    <t>CRS_FEAT003_002</t>
+  </si>
+  <si>
+    <t>in requirement description u should mention that the restaurant will be shown according to user zone</t>
+  </si>
+  <si>
+    <t>mention that the user will see the zone restaurant only</t>
+  </si>
+  <si>
+    <t>RVW-016</t>
+  </si>
+  <si>
+    <t>CRS_FEAT003_003</t>
+  </si>
+  <si>
+    <t>CRS_FEAT004_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> requiremt description need to be more clear </t>
+  </si>
+  <si>
+    <t>The requirement description must be clear, concise, and easily understandable to ensure that all stakeholders can interpret it correctly.</t>
+  </si>
+  <si>
+    <t>the requirement is pending ,till customer send siq answer</t>
+  </si>
+  <si>
+    <t>CRS_FEAT005_001</t>
+  </si>
+  <si>
+    <t>CRS_FEAT005_002</t>
+  </si>
+  <si>
+    <t>RVW-017</t>
+  </si>
+  <si>
+    <t>RVW-018</t>
+  </si>
+  <si>
+    <t>RVW-019</t>
+  </si>
+  <si>
+    <t>RVW-020</t>
+  </si>
+  <si>
+    <t>RVW-021</t>
+  </si>
+  <si>
+    <t>RVW-022</t>
+  </si>
+  <si>
+    <t>RVW-023</t>
+  </si>
+  <si>
+    <t>CRS_FEAT006_001</t>
+  </si>
+  <si>
+    <t>CRS_FEAT006_002</t>
+  </si>
+  <si>
+    <t>CRS_FEAT006_003</t>
+  </si>
+  <si>
+    <t>CRS_FEAT006_004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">requirement is not completed </t>
+  </si>
+  <si>
+    <t>RVW-024</t>
+  </si>
+  <si>
+    <t>RVW-025</t>
+  </si>
+  <si>
+    <t>RVW-026</t>
+  </si>
+  <si>
+    <t>RVW-027</t>
+  </si>
+  <si>
+    <t>CRS_FEAT007_001</t>
+  </si>
+  <si>
+    <t>CRS_FEAT007_002</t>
+  </si>
+  <si>
+    <t>CRS_FEAT007_003</t>
+  </si>
+  <si>
+    <t>CRS_FEAT008_001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -164,29 +306,34 @@
       <sz val="16"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="17"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color indexed="13"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -194,8 +341,27 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,8 +386,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF88CCFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -348,53 +520,285 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFA5A5A5"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFA5A5A5"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFA5A5A5"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA5A5A5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFA5A5A5"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFA5A5A5"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA5A5A5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+  <cellXfs count="37">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="18"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="15"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="17"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="16"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="18"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="15"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="17"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="16"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="18"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="15"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="17"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="16"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
@@ -1600,31 +2004,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21.45" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="29.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="29.1640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="44.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.21875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="44.1640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" style="1" customWidth="1"/>
     <col min="11" max="15" width="11.6640625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="8.88671875" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.88671875" style="1"/>
+    <col min="16" max="16" width="8.83203125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="26.85" customHeight="1">
+    <row r="1" spans="1:15" ht="26.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1661,7 +2065,7 @@
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
     </row>
-    <row r="2" spans="1:15" ht="70.2" customHeight="1">
+    <row r="2" spans="1:15" ht="70.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>10</v>
       </c>
@@ -1698,7 +2102,7 @@
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
     </row>
-    <row r="3" spans="1:15" ht="79.2" customHeight="1">
+    <row r="3" spans="1:15" ht="79.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>12</v>
       </c>
@@ -1735,7 +2139,7 @@
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
     </row>
-    <row r="4" spans="1:15" ht="46.2" customHeight="1">
+    <row r="4" spans="1:15" ht="46.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>14</v>
       </c>
@@ -1772,7 +2176,7 @@
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
     </row>
-    <row r="5" spans="1:15" ht="61.2" customHeight="1">
+    <row r="5" spans="1:15" ht="61.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>15</v>
       </c>
@@ -1809,7 +2213,7 @@
       <c r="N5" s="14"/>
       <c r="O5" s="14"/>
     </row>
-    <row r="6" spans="1:15" s="17" customFormat="1" ht="75" customHeight="1">
+    <row r="6" spans="1:15" s="17" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>31</v>
       </c>
@@ -1846,7 +2250,7 @@
       <c r="N6" s="16"/>
       <c r="O6" s="16"/>
     </row>
-    <row r="7" spans="1:15" ht="50.4" customHeight="1">
+    <row r="7" spans="1:15" ht="50.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>32</v>
       </c>
@@ -1883,7 +2287,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" spans="1:15" ht="54" customHeight="1">
+    <row r="8" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>33</v>
       </c>
@@ -1920,7 +2324,7 @@
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
     </row>
-    <row r="9" spans="1:15" ht="58.2" customHeight="1">
+    <row r="9" spans="1:15" ht="58.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>37</v>
       </c>
@@ -1957,7 +2361,7 @@
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
     </row>
-    <row r="10" spans="1:15" ht="51" customHeight="1">
+    <row r="10" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>38</v>
       </c>
@@ -1994,79 +2398,731 @@
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
     </row>
-    <row r="11" spans="1:15" ht="26.85" customHeight="1">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
+    <row r="11" spans="1:15" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="25">
+        <v>45758</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>47</v>
+      </c>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
     </row>
-    <row r="12" spans="1:15" ht="26.85" customHeight="1">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
+    <row r="12" spans="1:15" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="25">
+        <v>45758</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
     </row>
-    <row r="13" spans="1:15" ht="26.85" customHeight="1">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
+    <row r="13" spans="1:15" ht="44" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="25">
+        <v>45758</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
     </row>
+    <row r="14" spans="1:15" ht="44" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="33">
+        <v>45758</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="J14" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+    </row>
+    <row r="15" spans="1:15" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="33">
+        <v>45758</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="1:15" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="33">
+        <v>45758</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="I16" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+    </row>
+    <row r="17" spans="1:15" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="33">
+        <v>45758</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="I17" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+    </row>
+    <row r="18" spans="1:15" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="33">
+        <v>45758</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="H18" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="1:15" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="33">
+        <v>45758</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="I19" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+    </row>
+    <row r="20" spans="1:15" ht="38" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="33">
+        <v>45758</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="33">
+        <v>45758</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="H21" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+    </row>
+    <row r="22" spans="1:15" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="33">
+        <v>45758</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="H22" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="I22" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+    </row>
+    <row r="23" spans="1:15" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="33">
+        <v>45758</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G23" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="H23" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="I23" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="J23" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+    </row>
+    <row r="24" spans="1:15" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="33">
+        <v>45758</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="H24" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="I24" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="J24" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+    </row>
+    <row r="25" spans="1:15" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="33">
+        <v>45758</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G25" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="H25" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="I25" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+    </row>
+    <row r="26" spans="1:15" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" s="33">
+        <v>45758</v>
+      </c>
+      <c r="C26" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G26" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="H26" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="I26" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+    </row>
+    <row r="27" spans="1:15" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="33">
+        <v>45758</v>
+      </c>
+      <c r="C27" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G27" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="H27" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="I27" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+    </row>
+    <row r="28" spans="1:15" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="33">
+        <v>45758</v>
+      </c>
+      <c r="C28" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G28" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="H28" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="I28" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="J28" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+    </row>
+    <row r="29" spans="1:15" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A13 D1:D13">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="1" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="24" priority="31" stopIfTrue="1">
       <formula>NOT(ISBLANK(A1))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J13">
-    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="J1:J13 J15:J29">
+    <cfRule type="cellIs" dxfId="23" priority="33" stopIfTrue="1" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="33" stopIfTrue="1" operator="equal">
       <formula>"Approved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="33" stopIfTrue="1" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="34" stopIfTrue="1" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A17 A19">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="6" stopIfTrue="1">
+      <formula>NOT(ISBLANK(A17))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4" stopIfTrue="1">
+      <formula>NOT(ISBLANK(A21))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3" stopIfTrue="1">
+      <formula>NOT(ISBLANK(A22))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="2" stopIfTrue="1">
+      <formula>NOT(ISBLANK(A23))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A24:A29">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1" stopIfTrue="1">
+      <formula>NOT(ISBLANK(A24))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J13 J15:J29" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"In Progress,Pending,Completed,Approved,Rejected"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>